<commit_message>
finished adding GSD to summer samples
</commit_message>
<xml_diff>
--- a/GSD/Water Samples/LaJara_LISST_GSD_Summer2022.xlsx
+++ b/GSD/Water Samples/LaJara_LISST_GSD_Summer2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GSD\Water Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E331A614-FFDC-44C8-BC79-39278A5A5AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95445C73-8DC8-49B4-87F6-3A54FF9E0527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{5952B5DA-6B13-43D1-9193-1BE03F62DE4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
@@ -921,6 +921,18 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -931,18 +943,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29D726E-679A-4D28-8473-A292BA6CFD16}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,10 +1328,10 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="50"/>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1879,10 +1879,10 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="46"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="1" t="s">
         <v>0</v>
       </c>
@@ -2512,10 +2512,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="46"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
@@ -2933,10 +2933,10 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="46"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
@@ -3264,10 +3264,10 @@
     </row>
     <row r="68" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="43" t="s">
+      <c r="A69" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="B69" s="44"/>
+      <c r="B69" s="48"/>
       <c r="C69" s="30" t="s">
         <v>0</v>
       </c>
@@ -3676,10 +3676,10 @@
     </row>
     <row r="82" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="43" t="s">
+      <c r="A83" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B83" s="44"/>
+      <c r="B83" s="48"/>
       <c r="C83" s="30" t="s">
         <v>0</v>
       </c>
@@ -4112,10 +4112,10 @@
     </row>
     <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="43" t="s">
+      <c r="A98" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B98" s="44"/>
+      <c r="B98" s="48"/>
       <c r="C98" s="30" t="s">
         <v>0</v>
       </c>
@@ -4395,10 +4395,10 @@
     </row>
     <row r="110" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="111" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="43" t="s">
+      <c r="A111" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="B111" s="44"/>
+      <c r="B111" s="48"/>
       <c r="C111" s="30" t="s">
         <v>0</v>
       </c>
@@ -4588,10 +4588,10 @@
     </row>
     <row r="119" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="43" t="s">
+      <c r="A120" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B120" s="44"/>
+      <c r="B120" s="48"/>
       <c r="C120" s="30" t="s">
         <v>0</v>
       </c>
@@ -4974,10 +4974,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
@@ -4998,7 +4998,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="45">
         <v>44776.626388888886</v>
       </c>
       <c r="C3" s="4">
@@ -5021,7 +5021,7 @@
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="44">
         <v>44776.636805555558</v>
       </c>
       <c r="C4" s="7">
@@ -5044,7 +5044,7 @@
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="44">
         <v>44776.647222222222</v>
       </c>
       <c r="C5" s="7">
@@ -5068,7 +5068,7 @@
         <f>A5+1</f>
         <v>4</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="44">
         <v>44776.657638888886</v>
       </c>
       <c r="C6" s="7">
@@ -5092,7 +5092,7 @@
         <f t="shared" ref="A7:A9" si="0">A6+1</f>
         <v>5</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="44">
         <v>44776.668055555558</v>
       </c>
       <c r="C7" s="7">
@@ -5116,7 +5116,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="44">
         <v>44776.678472222222</v>
       </c>
       <c r="C8" s="7">
@@ -5140,7 +5140,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="48">
+      <c r="B9" s="44">
         <v>44776.688888888886</v>
       </c>
       <c r="C9" s="7">
@@ -5163,7 +5163,7 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="44">
         <v>44776.709722222222</v>
       </c>
       <c r="C10" s="7">
@@ -5186,7 +5186,7 @@
       <c r="A11" s="6">
         <v>11</v>
       </c>
-      <c r="B11" s="48">
+      <c r="B11" s="44">
         <v>44776.730555555558</v>
       </c>
       <c r="C11" s="7">
@@ -5209,7 +5209,7 @@
       <c r="A12" s="34">
         <v>12</v>
       </c>
-      <c r="B12" s="48">
+      <c r="B12" s="44">
         <v>44776.740972222222</v>
       </c>
       <c r="C12" s="7">
@@ -5232,7 +5232,7 @@
       <c r="A13" s="6">
         <v>13</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="44">
         <v>44776.751388888886</v>
       </c>
       <c r="C13" s="7">
@@ -5256,7 +5256,7 @@
         <f t="shared" ref="A14:A24" si="1">A13+1</f>
         <v>14</v>
       </c>
-      <c r="B14" s="48">
+      <c r="B14" s="44">
         <v>44776.761805555558</v>
       </c>
       <c r="C14" s="7">
@@ -5280,7 +5280,7 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B15" s="48">
+      <c r="B15" s="44">
         <v>44776.772222222222</v>
       </c>
       <c r="C15" s="7">
@@ -5304,7 +5304,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="44">
         <v>44776.782638888886</v>
       </c>
       <c r="C16" s="7">
@@ -5328,7 +5328,7 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B17" s="48">
+      <c r="B17" s="44">
         <v>44776.793055555558</v>
       </c>
       <c r="C17" s="7">
@@ -5352,7 +5352,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B18" s="48">
+      <c r="B18" s="44">
         <v>44776.803472222222</v>
       </c>
       <c r="C18" s="7">
@@ -5376,7 +5376,7 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B19" s="48">
+      <c r="B19" s="44">
         <v>44776.813888888886</v>
       </c>
       <c r="C19" s="7">
@@ -5400,7 +5400,7 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B20" s="48">
+      <c r="B20" s="44">
         <v>44776.824305555558</v>
       </c>
       <c r="C20" s="7">
@@ -5424,7 +5424,7 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B21" s="48">
+      <c r="B21" s="44">
         <v>44776.834722222222</v>
       </c>
       <c r="C21" s="7">
@@ -5448,7 +5448,7 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B22" s="48">
+      <c r="B22" s="44">
         <v>44776.845138888886</v>
       </c>
       <c r="C22" s="7">
@@ -5472,7 +5472,7 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B23" s="48">
+      <c r="B23" s="44">
         <v>44776.855555555558</v>
       </c>
       <c r="C23" s="7">
@@ -5496,7 +5496,7 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B24" s="50">
+      <c r="B24" s="46">
         <v>44776.865972222222</v>
       </c>
       <c r="C24" s="13">
@@ -5528,7 +5528,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5541,10 +5541,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
@@ -5565,7 +5565,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="43">
         <v>44781.571527777778</v>
       </c>
       <c r="C3" s="4">
@@ -5588,7 +5588,7 @@
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="43">
         <v>44781.581944444442</v>
       </c>
       <c r="C4" s="7">
@@ -5635,7 +5635,7 @@
         <f>A5+1</f>
         <v>4</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="43">
         <v>44781.602777777778</v>
       </c>
       <c r="C6" s="7">
@@ -5659,7 +5659,7 @@
         <f t="shared" ref="A7:A9" si="0">A6+1</f>
         <v>5</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="43">
         <v>44781.613194444442</v>
       </c>
       <c r="C7" s="7">
@@ -5707,7 +5707,7 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="43">
         <v>44781.640972222223</v>
       </c>
       <c r="C9" s="7">
@@ -5753,7 +5753,7 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="43">
         <v>44781.675694444442</v>
       </c>
       <c r="C11" s="7">
@@ -5776,7 +5776,7 @@
       <c r="A12" s="34">
         <v>11</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="43">
         <v>44781.686111111114</v>
       </c>
       <c r="C12" s="7">
@@ -5823,7 +5823,7 @@
         <f t="shared" ref="A14:A24" si="1">A13+1</f>
         <v>14</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="43">
         <v>44781.706944444442</v>
       </c>
       <c r="C14" s="7">
@@ -5871,7 +5871,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="43">
         <v>44781.727777777778</v>
       </c>
       <c r="C16" s="7">
@@ -5943,7 +5943,7 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="43">
         <v>44781.759027777778</v>
       </c>
       <c r="C19" s="7">
@@ -6095,7 +6095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFEFC0C2-126A-40CD-B1C8-F2F6F391675D}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -6110,10 +6110,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="47" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="48"/>
       <c r="C2" s="30" t="s">
         <v>0</v>
       </c>

</xml_diff>